<commit_message>
GSYE-681: Added support for SCMStorage strategy in the CDS. Modified schema in order to support the SCMStorage strategy.
</commit_message>
<xml_diff>
--- a/tests/fixtures/community_datasheet_alt.xlsx
+++ b/tests/fixtures/community_datasheet_alt.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="General settings" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="49">
   <si>
     <t xml:space="preserve">start_date</t>
   </si>
@@ -157,15 +157,6 @@
   </si>
   <si>
     <t xml:space="preserve">Battery_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Capacity [kWh]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Minimum allowed SoC [-]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maximum power [kW]</t>
   </si>
   <si>
     <t xml:space="preserve">Battery 1</t>
@@ -332,7 +323,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C1:E8 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -472,8 +463,8 @@
   </sheetPr>
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L8" activeCellId="1" sqref="C1:E8 L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -683,7 +674,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C1:E8 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -782,7 +773,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C1:E8 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -900,8 +891,8 @@
   </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -921,49 +912,31 @@
       <c r="B1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>46</v>
-      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="4" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="D2" s="4" t="n">
-        <v>10</v>
-      </c>
-      <c r="E2" s="4" t="n">
-        <v>0.005</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="4" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D3" s="4" t="n">
-        <v>10</v>
-      </c>
-      <c r="E3" s="4" t="n">
-        <v>0.005</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4"/>
@@ -1019,7 +992,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C1:E8 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1030,7 +1003,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>36</v>
@@ -1041,13 +1014,13 @@
     </row>
     <row r="2" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>